<commit_message>
fill week and update today
</commit_message>
<xml_diff>
--- a/04.03-29.03.xlsx
+++ b/04.03-29.03.xlsx
@@ -97,7 +97,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,14 +136,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -258,14 +250,13 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="3" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="5"/>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -275,19 +266,19 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -578,7 +569,7 @@
   <dimension ref="B2:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="H30" sqref="H30:H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,108 +609,108 @@
       <c r="C3" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>5</v>
       </c>
       <c r="E3" s="1">
         <v>0.625</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="6">
         <v>4.5</v>
       </c>
       <c r="G3" s="1">
         <v>0.5</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="6">
         <v>7.5</v>
       </c>
       <c r="I3" s="1">
         <v>0.45833333333333331</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3" s="6">
         <v>8</v>
       </c>
       <c r="K3" s="1"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="8"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="7"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>
       <c r="C4" s="1">
         <v>0.79166666666666663</v>
       </c>
-      <c r="D4" s="7"/>
+      <c r="D4" s="6"/>
       <c r="E4" s="1">
         <v>0.8125</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="6"/>
       <c r="G4" s="1">
         <v>0.8125</v>
       </c>
-      <c r="H4" s="7"/>
+      <c r="H4" s="6"/>
       <c r="I4" s="1">
         <v>0.79166666666666663</v>
       </c>
-      <c r="J4" s="7"/>
+      <c r="J4" s="6"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="8"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="7"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="9">
         <v>5</v>
       </c>
       <c r="E6" s="1">
         <v>0.61458333333333337</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="9">
         <v>4</v>
       </c>
       <c r="G6" s="1">
         <v>0.5</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="9">
         <v>7.5</v>
       </c>
       <c r="I6" s="1">
         <v>0.45833333333333331</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="8">
         <v>8</v>
       </c>
       <c r="K6" s="1"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="8">
+      <c r="L6" s="8"/>
+      <c r="M6" s="7">
         <v>24.5</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="9"/>
+      <c r="B7" s="8"/>
       <c r="C7" s="1">
         <v>0.79166666666666663</v>
       </c>
-      <c r="D7" s="11"/>
+      <c r="D7" s="9"/>
       <c r="E7" s="1">
         <v>0.78125</v>
       </c>
-      <c r="F7" s="11"/>
+      <c r="F7" s="9"/>
       <c r="G7" s="1">
         <v>0.8125</v>
       </c>
-      <c r="H7" s="11"/>
+      <c r="H7" s="9"/>
       <c r="I7" s="1">
         <v>0.79166666666666663</v>
       </c>
-      <c r="J7" s="9"/>
+      <c r="J7" s="8"/>
       <c r="K7" s="1"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="7"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
@@ -753,106 +744,120 @@
       <c r="C11" s="1">
         <v>0.67708333333333337</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="6">
         <v>2.5</v>
       </c>
       <c r="E11" s="1">
         <v>0.625</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="6">
         <v>4.5</v>
       </c>
       <c r="G11" s="1">
         <v>0.5</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="13">
         <v>7.5</v>
       </c>
       <c r="I11" s="1">
         <v>0.55208333333333337</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="6">
         <v>6.5</v>
       </c>
-      <c r="K11" s="1"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="8"/>
+      <c r="K11" s="1">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="L11" s="6">
+        <v>6.5</v>
+      </c>
+      <c r="M11" s="7"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="10"/>
       <c r="C12" s="1">
         <v>0.78125</v>
       </c>
-      <c r="D12" s="7"/>
+      <c r="D12" s="6"/>
       <c r="E12" s="1">
         <v>0.8125</v>
       </c>
-      <c r="F12" s="7"/>
+      <c r="F12" s="6"/>
       <c r="G12" s="1">
         <v>0.82291666666666663</v>
       </c>
-      <c r="H12" s="12"/>
+      <c r="H12" s="13"/>
       <c r="I12" s="1">
         <v>0.82291666666666663</v>
       </c>
-      <c r="J12" s="7"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="8"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="1">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="L12" s="6"/>
+      <c r="M12" s="7"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="1">
         <v>0.67708333333333337</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="9">
         <v>2.5</v>
       </c>
       <c r="E14" s="1">
         <v>0.625</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="9">
         <v>4.5</v>
       </c>
       <c r="G14" s="1">
         <v>0.51041666666666663</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="8">
         <v>7.5</v>
       </c>
       <c r="I14" s="1">
         <v>0.55208333333333337</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J14" s="8">
         <v>5.5</v>
       </c>
-      <c r="K14" s="6"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="8"/>
+      <c r="K14" s="1">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="L14" s="8">
+        <v>6.5</v>
+      </c>
+      <c r="M14" s="7">
+        <v>26.5</v>
+      </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="9"/>
+      <c r="B15" s="8"/>
       <c r="C15" s="1">
         <v>0.78125</v>
       </c>
-      <c r="D15" s="11"/>
+      <c r="D15" s="9"/>
       <c r="E15" s="1">
         <v>0.8125</v>
       </c>
-      <c r="F15" s="11"/>
+      <c r="F15" s="9"/>
       <c r="G15" s="1">
         <v>0.82291666666666663</v>
       </c>
-      <c r="H15" s="9"/>
+      <c r="H15" s="8"/>
       <c r="I15" s="1">
         <v>0.82291666666666663</v>
       </c>
-      <c r="J15" s="9"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="1">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="L15" s="8"/>
+      <c r="M15" s="7"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C18" s="2">
@@ -884,60 +889,60 @@
         <v>1</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="D19" s="7"/>
+      <c r="D19" s="6"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="7"/>
+      <c r="F19" s="6"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="7"/>
+      <c r="H19" s="6"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="7"/>
+      <c r="J19" s="6"/>
       <c r="K19" s="1"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="8"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="7"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="10"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="7"/>
+      <c r="D20" s="6"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="7"/>
+      <c r="F20" s="6"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="7"/>
+      <c r="H20" s="6"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="7"/>
+      <c r="J20" s="6"/>
       <c r="K20" s="1"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="8"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="7"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="D22" s="9"/>
+      <c r="D22" s="8"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="9"/>
+      <c r="F22" s="8"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="9"/>
+      <c r="H22" s="8"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="9"/>
+      <c r="J22" s="8"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="7"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="9"/>
+      <c r="B23" s="8"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="9"/>
+      <c r="D23" s="8"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="9"/>
+      <c r="F23" s="8"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="9"/>
+      <c r="H23" s="8"/>
       <c r="I23" s="1"/>
-      <c r="J23" s="9"/>
+      <c r="J23" s="8"/>
       <c r="K23" s="1"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="7"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C26" s="2">
@@ -968,64 +973,156 @@
       <c r="B27" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="7"/>
-      <c r="M27" s="8"/>
+      <c r="C27" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="D27" s="6">
+        <v>5</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="F27" s="11">
+        <v>4.5</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="H27" s="11">
+        <v>8</v>
+      </c>
+      <c r="I27" s="1">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="J27" s="6">
+        <v>4.5</v>
+      </c>
+      <c r="K27" s="1">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="L27" s="6">
+        <v>4.5</v>
+      </c>
+      <c r="M27" s="7">
+        <v>26.5</v>
+      </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="10"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="7"/>
-      <c r="M28" s="8"/>
+      <c r="C28" s="1">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D28" s="6"/>
+      <c r="E28" s="1">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="F28" s="12"/>
+      <c r="G28" s="1">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="H28" s="12"/>
+      <c r="I28" s="1">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="J28" s="6"/>
+      <c r="K28" s="1">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="L28" s="6"/>
+      <c r="M28" s="7"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="11"/>
+      <c r="C30" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="D30" s="9">
+        <v>5</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="F30" s="8">
+        <v>4.5</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="H30" s="9">
+        <v>8</v>
+      </c>
       <c r="I30" s="1"/>
-      <c r="J30" s="9"/>
+      <c r="J30" s="8"/>
       <c r="K30" s="1"/>
-      <c r="L30" s="11"/>
-      <c r="M30" s="8"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="7"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B31" s="9"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="11"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="1">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D31" s="9"/>
+      <c r="E31" s="1">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="F31" s="8"/>
+      <c r="G31" s="1">
+        <v>0.8125</v>
+      </c>
+      <c r="H31" s="9"/>
       <c r="I31" s="1"/>
-      <c r="J31" s="9"/>
+      <c r="J31" s="8"/>
       <c r="K31" s="1"/>
-      <c r="L31" s="11"/>
-      <c r="M31" s="8"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="56">
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="J11:J12"/>
     <mergeCell ref="J27:J28"/>
     <mergeCell ref="L27:L28"/>
     <mergeCell ref="M27:M28"/>
@@ -1040,48 +1137,6 @@
     <mergeCell ref="D27:D28"/>
     <mergeCell ref="F27:F28"/>
     <mergeCell ref="H27:H28"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="M19:M20"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="J19:J20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>